<commit_message>
Tkinter working UI Update
</commit_message>
<xml_diff>
--- a/Hornerstown S9000.xlsx
+++ b/Hornerstown S9000.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wblankenship\Documents\GitHub\SPT-Builder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF92E83E-663B-4DFD-87CD-DE7F1726615D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE83FB5-3E80-4335-AE99-3196BB3D3064}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D2F1E244-0055-49E9-BA99-E37AFD162BFC}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="26">
   <si>
     <t>SPARE</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t xml:space="preserve">67292 MVAR </t>
+  </si>
+  <si>
+    <t>SPARE&amp;</t>
   </si>
 </sst>
 </file>
@@ -463,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A9C7EB-CAA4-4DB0-AECE-FAF550B5EE12}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,7 +751,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Updates to config generator and tkinter test script
</commit_message>
<xml_diff>
--- a/Hornerstown S9000.xlsx
+++ b/Hornerstown S9000.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wblankenship\Documents\GitHub\SPT-Builder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE83FB5-3E80-4335-AE99-3196BB3D3064}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC66696D-07A4-471C-9D0A-844F7509BE32}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D2F1E244-0055-49E9-BA99-E37AFD162BFC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D2F1E244-0055-49E9-BA99-E37AFD162BFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="50">
   <si>
     <t>SPARE</t>
   </si>
@@ -90,25 +90,97 @@
     <t>H60-3 LBSW</t>
   </si>
   <si>
-    <t>SPARE-SCAN1</t>
-  </si>
-  <si>
-    <t>BATTERY</t>
-  </si>
-  <si>
-    <t>67291 MW</t>
-  </si>
-  <si>
-    <t>67291 MVAR</t>
-  </si>
-  <si>
-    <t>67292 MW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">67292 MVAR </t>
-  </si>
-  <si>
-    <t>SPARE&amp;</t>
+    <t>BK 1 VCB</t>
+  </si>
+  <si>
+    <t>47417 VCB</t>
+  </si>
+  <si>
+    <t>BT VCB</t>
+  </si>
+  <si>
+    <t>BK 2 VCB</t>
+  </si>
+  <si>
+    <t>47418 VCB</t>
+  </si>
+  <si>
+    <t>47419 VCB</t>
+  </si>
+  <si>
+    <t>47416 VCB</t>
+  </si>
+  <si>
+    <t>47415 VCB</t>
+  </si>
+  <si>
+    <t>DIAL IN ACCESS</t>
+  </si>
+  <si>
+    <t>BK 1 CKT INT CI-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPARE </t>
+  </si>
+  <si>
+    <t>I87 LBSW</t>
+  </si>
+  <si>
+    <t>NO 6 LBSW</t>
+  </si>
+  <si>
+    <t>A53 LBSW</t>
+  </si>
+  <si>
+    <t>BK 1 ALRM</t>
+  </si>
+  <si>
+    <t>BK 2 ALRM</t>
+  </si>
+  <si>
+    <t>CAP 1 VCB</t>
+  </si>
+  <si>
+    <t>DX RELAY FAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOSS OF POTENTIAL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BK 1 CKT INT CI-2/SEL TRBL  </t>
+  </si>
+  <si>
+    <t>UNDEFINED</t>
+  </si>
+  <si>
+    <t>BK 1 MW</t>
+  </si>
+  <si>
+    <t>BK 1 MVAR</t>
+  </si>
+  <si>
+    <t>BK 2 MW</t>
+  </si>
+  <si>
+    <t>BK 2 MVAR</t>
+  </si>
+  <si>
+    <t>47416 phase A amps</t>
+  </si>
+  <si>
+    <t>47416 phase B amps</t>
+  </si>
+  <si>
+    <t>47416 phase C amps</t>
+  </si>
+  <si>
+    <t>47417 phase A amps</t>
+  </si>
+  <si>
+    <t>47417 phase B amps</t>
+  </si>
+  <si>
+    <t>47417 phase C amps</t>
   </si>
 </sst>
 </file>
@@ -144,9 +216,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -466,21 +537,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A9C7EB-CAA4-4DB0-AECE-FAF550B5EE12}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.28515625" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -489,16 +560,15 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1"/>
-      <c r="F1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -507,15 +577,15 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -524,15 +594,15 @@
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -541,15 +611,15 @@
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -558,15 +628,15 @@
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -575,15 +645,15 @@
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -592,15 +662,15 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -609,15 +679,15 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -625,13 +695,16 @@
       <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="F9" t="s">
+      <c r="D9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
@@ -639,11 +712,14 @@
       <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="F10" t="s">
+      <c r="D10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -653,8 +729,11 @@
       <c r="C11" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -664,8 +743,11 @@
       <c r="C12" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -676,9 +758,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
@@ -687,9 +769,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
@@ -698,9 +780,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
@@ -711,7 +793,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
@@ -719,7 +801,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
@@ -727,7 +809,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
@@ -735,7 +817,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
@@ -743,7 +825,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
@@ -751,7 +833,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
@@ -759,7 +841,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -767,7 +849,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
@@ -775,7 +857,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
@@ -783,7 +865,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -791,7 +873,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
@@ -807,34 +889,34 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>0</v>
-      </c>
-      <c r="G34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H34" t="s">
@@ -843,9 +925,9 @@
     </row>
     <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>0</v>
-      </c>
-      <c r="G35" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H35" t="s">
@@ -854,37 +936,37 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>